<commit_message>
HITO: Funcionó prueba con Juan
</commit_message>
<xml_diff>
--- a/backend/mock_data.xlsx
+++ b/backend/mock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46016</v>
+        <v>46017</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -511,7 +511,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46016</v>
+        <v>46017</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -546,36 +546,106 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46017</v>
+        <v>46018</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>TKT-M1-01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Juan Perez</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>XY-9999</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Cliente Manana</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Ruta 66 km 10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Mantenimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>46018</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>TKT-003</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Maria Gonzalez</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Juan Perez</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>EF-9012</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Chile Trucks</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Panamericana Norte 5000</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Desinstalacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>46016</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TKT-OLD-01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Juan Perez</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ZZ-0000</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Old Task</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Somewhere</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Audit</t>
         </is>
       </c>
     </row>

</xml_diff>